<commit_message>
Add high-low in the xlsx file
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="總成績" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="23">
   <si>
     <t>Isolation</t>
   </si>
@@ -99,6 +99,10 @@
   </si>
   <si>
     <t>背號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High-Low</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +153,11 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +176,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,8 +196,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,8 +231,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="35">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -218,6 +244,14 @@
     <cellStyle name="已瀏覽過的超連結" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -227,6 +261,14 @@
     <cellStyle name="超連結" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="33" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -555,15 +597,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA2"/>
+  <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BW10" sqref="BW10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:79">
+    <row r="1" spans="1:84">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -652,31 +694,38 @@
       <c r="BJ1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="BK1" s="5"/>
-      <c r="BL1" s="5"/>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+      <c r="BM1" s="7"/>
+      <c r="BN1" s="7"/>
       <c r="BO1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP1" s="4"/>
+      <c r="BQ1" s="4"/>
+      <c r="BR1" s="4"/>
+      <c r="BS1" s="4"/>
+      <c r="BT1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="BP1" s="5"/>
-      <c r="BQ1" s="5"/>
-      <c r="BR1" s="5"/>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="5"/>
+      <c r="BV1" s="5"/>
+      <c r="BW1" s="5"/>
+      <c r="BX1" s="5"/>
+      <c r="BY1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="BU1" s="4"/>
-      <c r="BV1" s="4"/>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4"/>
+      <c r="CA1" s="4"/>
+      <c r="CB1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BX1" s="5"/>
-      <c r="BY1" s="5"/>
-      <c r="BZ1" s="5"/>
-      <c r="CA1" s="5"/>
+      <c r="CC1" s="5"/>
+      <c r="CD1" s="5"/>
+      <c r="CE1" s="5"/>
+      <c r="CF1" s="5"/>
     </row>
-    <row r="2" spans="1:79">
+    <row r="2" spans="1:84">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -897,28 +946,51 @@
         <v>3</v>
       </c>
       <c r="BV2" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="BW2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BX2" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="BY2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="BZ2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CA2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CB2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="CF2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="CB1:CF1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="BT1:BX1"/>
     <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="BT1:BV1"/>
+    <mergeCell ref="BY1:CA1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="L1:P1"/>
@@ -926,13 +998,6 @@
     <mergeCell ref="V1:Z1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BW1:CA1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BE1:BI1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>